<commit_message>
Optimized the log module and added a use-case data processing factory
</commit_message>
<xml_diff>
--- a/Data/UITestData/test_data.xlsx
+++ b/Data/UITestData/test_data.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13920"/>
+    <workbookView windowWidth="28000" windowHeight="11940"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="HomePage" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
   <si>
     <t>CaseID</t>
   </si>
@@ -36,24 +36,169 @@
     <t>Excepted</t>
   </si>
   <si>
+    <t>BGM-01-001</t>
+  </si>
+  <si>
     <t>用户注册-正常测试-用户注册功能</t>
   </si>
   <si>
     <t>检查用户注册功能是否正常</t>
+  </si>
+  <si>
+    <t>1、输入格式正确用户名
+2、输入格式正确邮箱
+3、输入格式正确密码
+4、输入与密码一致的确认密码
+5、输入正确验证码
+6、点击注册</t>
+  </si>
+  <si>
+    <t>{'UserName' : 'test555', 'Email' : 'test@qq.com', 'Password' : 'test@123', 'Confirm_Password' : 'test@123'}</t>
+  </si>
+  <si>
+    <t>注册成功</t>
+  </si>
+  <si>
+    <t>BGM-01-002</t>
+  </si>
+  <si>
+    <t>用户注册-异常测试-用户名为空</t>
+  </si>
+  <si>
+    <t>检查用户名必填限制功能</t>
+  </si>
+  <si>
+    <t>1、不输入用户名
+2、输入格式正确邮箱
+3、输入格式正确密码
+4、输入与密码一致的确认密码
+5、输入正确验证码
+6、点击注册</t>
+  </si>
+  <si>
+    <t>{'UserName' : '', 'Email' : 'test@qq.com', 'Password' : 'test@123', 'Confirm_Password' : 'test@123'}</t>
+  </si>
+  <si>
+    <t>注册失败，用户名下方提示“这是必填内容”</t>
+  </si>
+  <si>
+    <t>BGM-01-003</t>
+  </si>
+  <si>
+    <t>用户注册-异常测试-邮箱为空</t>
+  </si>
+  <si>
+    <t>检查邮箱必填限制功能</t>
+  </si>
+  <si>
+    <t>1、输入格式正确用户名
+2、邮箱为空
+3、输入格式正确密码
+4、输入与密码一致的确认密码
+5、输入正确验证码
+6、点击注册</t>
+  </si>
+  <si>
+    <t>{'UserName' : 'test555', 'Email' : '', 'Password' : 'test@123', 'Confirm_Password' : 'test@123'}</t>
+  </si>
+  <si>
+    <t>注册失败，邮箱下方提示“这是必填内容”</t>
+  </si>
+  <si>
+    <t>BGM-01-004</t>
+  </si>
+  <si>
+    <t>用户注册-异常测试-密码为空</t>
+  </si>
+  <si>
+    <t>检查密码必填限制功能</t>
+  </si>
+  <si>
+    <t>1、输入格式正确用户名
+2、输入格式正确邮箱
+3、密码为空
+4、输入与密码一致的确认密码
+5、输入正确验证码
+6、点击注册</t>
+  </si>
+  <si>
+    <t>{'UserName' : 'test555', 'Email' : '', 'Password' : '', 'Confirm_Password' : 'test@123'}</t>
+  </si>
+  <si>
+    <t>注册失败，密码下方提示“这是必填内容”</t>
+  </si>
+  <si>
+    <t>用户注册-异常测试-确认密码为空</t>
+  </si>
+  <si>
+    <t>检查确认密码必填限制功能</t>
+  </si>
+  <si>
+    <t>1、输入格式正确用户名
+2、输入格式正确邮箱
+3、输入格式正确密码
+4、确认密码为空
+5、输入正确验证码
+6、点击注册</t>
+  </si>
+  <si>
+    <t>{'UserName' : 'test555', 'Email' : 'test@qq.com', 'Password' : 'test@123', 'Confirm_Password' : ''}</t>
+  </si>
+  <si>
+    <t>注册失败，确认密码下方提示“这是必填内容”</t>
+  </si>
+  <si>
+    <t>BGM-01-005</t>
+  </si>
+  <si>
+    <t>用户注册-异常测试-验证码为空</t>
+  </si>
+  <si>
+    <t>检查验证码必填限制功能</t>
+  </si>
+  <si>
+    <t>1、输入格式正确用户名
+2、输入格式正确邮箱
+3、输入格式正确密码
+4、输入与密码一致的确认密码
+5、验证码为空
+6、点击注册</t>
+  </si>
+  <si>
+    <t>注册失败，验证码右侧提示“这是必填内容”</t>
+  </si>
+  <si>
+    <t>BGM-02-001</t>
+  </si>
+  <si>
+    <t>用户登录-正常测试-用户登录功能</t>
+  </si>
+  <si>
+    <t>检查用户登录功能是否正常</t>
   </si>
   <si>
     <t>1、输入格式正确用户名
 2、输入格式正确密码
-3、输入与密码一致的确认密码
-4、输入格式正确邮箱
-5、输入正确验证码
-6、点击注册</t>
-  </si>
-  <si>
-    <t>{'UserName' : 'test555','Password' : 'test@123','Confirm_Password' : 'test@123','Email' : 'test@qq.com'}</t>
-  </si>
-  <si>
-    <t>注册成功</t>
+3、输入正确验证码
+4、点击登录</t>
+  </si>
+  <si>
+    <t>{'UserName' : 'test555','Password' : 'test@123'}</t>
+  </si>
+  <si>
+    <t>BGM-02-002</t>
+  </si>
+  <si>
+    <t>用户登录-异常测试-用户名为空</t>
+  </si>
+  <si>
+    <t>检查用户名输入框必填限制功能</t>
+  </si>
+  <si>
+    <t>1、不输入用户名
+2、输入格式正确密码
+3、输入正确验证码
+4、点击登录</t>
   </si>
 </sst>
 </file>
@@ -61,12 +206,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,6 +220,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -83,12 +273,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -96,23 +318,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -126,17 +342,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,70 +357,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,19 +380,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -252,19 +482,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,19 +524,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,115 +542,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,6 +571,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -435,46 +611,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,6 +642,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -524,152 +676,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -680,6 +832,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1001,15 +1159,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="9.22321428571429" customWidth="1"/>
+    <col min="1" max="1" width="16.6696428571429" customWidth="1"/>
     <col min="2" max="3" width="21.1339285714286" customWidth="1"/>
     <col min="4" max="4" width="36.4553571428571" customWidth="1"/>
     <col min="5" max="5" width="37.1964285714286" customWidth="1"/>
@@ -1037,25 +1195,128 @@
       </c>
     </row>
     <row r="2" ht="114" customHeight="1" spans="1:6">
-      <c r="A2" s="2">
-        <v>1</v>
+      <c r="A2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" ht="121" customHeight="1" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" ht="118" customHeight="1" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" ht="113" customHeight="1" spans="1:6">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" ht="124" customHeight="1" spans="1:6">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" ht="115" customHeight="1" spans="1:6">
+      <c r="A7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="F7" s="5" t="s">
+        <v>39</v>
+      </c>
     </row>
+    <row r="8" ht="29" customHeight="1"/>
+    <row r="9" ht="29" customHeight="1"/>
+    <row r="10" ht="29" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1065,14 +1326,80 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="2" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="14.1339285714286" customWidth="1"/>
+    <col min="2" max="2" width="40.1785714285714" customWidth="1"/>
+    <col min="3" max="6" width="29.9017857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" ht="125" customHeight="1" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" ht="71" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>